<commit_message>
Commit my changes to the WRDS data
</commit_message>
<xml_diff>
--- a/Datasets/ESG_Formatted.xlsx
+++ b/Datasets/ESG_Formatted.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maralinetorres/Documents/GitHub/Predicting-Environmental-and-Social-Actions/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C040669-B13F-3E44-BDE6-A71EC8C1AFFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B132A0C-EB25-3B42-990B-1C5BE756EF6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15780" xr2:uid="{FE21AA8B-6B2A-B14E-8381-3F1748108412}"/>
+    <workbookView xWindow="-33220" yWindow="-5380" windowWidth="27640" windowHeight="15780" xr2:uid="{FE21AA8B-6B2A-B14E-8381-3F1748108412}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -446,13 +446,13 @@
   <dimension ref="A1:F192"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
     <col min="5" max="5" width="24.1640625" customWidth="1"/>
   </cols>

</xml_diff>